<commit_message>
Export XLSX from Google Sheet (entities)
</commit_message>
<xml_diff>
--- a/gsheet/xlsx/entities.xlsx
+++ b/gsheet/xlsx/entities.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1156" uniqueCount="900">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1159" uniqueCount="901">
   <si>
     <t>Person-ID</t>
   </si>
@@ -1999,6 +1999,12 @@
     <t>person_193</t>
   </si>
   <si>
+    <t>Hans Wilhelm</t>
+  </si>
+  <si>
+    <t>1037530217</t>
+  </si>
+  <si>
     <t>person_194</t>
   </si>
   <si>
@@ -2012,9 +2018,6 @@
   </si>
   <si>
     <t>Namensvariante</t>
-  </si>
-  <si>
-    <t>Geonames</t>
   </si>
   <si>
     <t>place_001</t>
@@ -3111,15 +3114,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:G62" displayName="Orteindex" name="Orteindex" id="2">
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:F62" displayName="Orteindex" name="Orteindex" id="2">
+  <tableColumns count="6">
     <tableColumn name="Ort-ID" id="1"/>
     <tableColumn name="Label [generiert, nicht manuell berarbeiten]" id="2"/>
     <tableColumn name="Name" id="3"/>
     <tableColumn name="Namensvariante" id="4"/>
-    <tableColumn name="Geonames" id="5"/>
-    <tableColumn name="Kategorie" id="6"/>
-    <tableColumn name="Bemerkungen" id="7"/>
+    <tableColumn name="Kategorie" id="5"/>
+    <tableColumn name="Bemerkungen" id="6"/>
   </tableColumns>
   <tableStyleInfo name="Orte-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
@@ -8094,7 +8096,9 @@
       <c r="H183" s="3" t="s">
         <v>625</v>
       </c>
-      <c r="I183" s="13"/>
+      <c r="I183" s="7" t="s">
+        <v>16</v>
+      </c>
       <c r="J183" s="8"/>
       <c r="K183" s="8"/>
     </row>
@@ -8222,13 +8226,19 @@
       </c>
       <c r="B189" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>,  (-)</v>
-      </c>
-      <c r="C189" s="6"/>
-      <c r="D189" s="3"/>
+        <v>Simler, Hans Wilhelm (-)</v>
+      </c>
+      <c r="C189" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D189" s="3" t="s">
+        <v>640</v>
+      </c>
       <c r="E189" s="15"/>
       <c r="F189" s="16"/>
-      <c r="G189" s="8"/>
+      <c r="G189" s="3" t="s">
+        <v>641</v>
+      </c>
       <c r="H189" s="3"/>
       <c r="I189" s="13"/>
       <c r="J189" s="8"/>
@@ -8236,7 +8246,7 @@
     </row>
     <row r="190" ht="22.5" customHeight="1">
       <c r="A190" s="3" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="B190" s="4" t="str">
         <f t="shared" si="1"/>
@@ -8254,7 +8264,7 @@
     </row>
     <row r="191" ht="22.5" customHeight="1">
       <c r="A191" s="3" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
       <c r="B191" s="4" t="str">
         <f t="shared" si="1"/>
@@ -8319,1071 +8329,1006 @@
     <col customWidth="1" min="2" max="2" width="30.63"/>
     <col customWidth="1" min="3" max="3" width="23.13"/>
     <col customWidth="1" min="4" max="4" width="17.75"/>
-    <col customWidth="1" min="5" max="5" width="22.13"/>
-    <col customWidth="1" min="6" max="6" width="22.25"/>
-    <col customWidth="1" min="7" max="7" width="25.13"/>
+    <col customWidth="1" min="5" max="5" width="22.25"/>
+    <col customWidth="1" min="6" max="6" width="25.13"/>
   </cols>
   <sheetData>
     <row r="1" ht="22.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>645</v>
+        <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" ht="22.5" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="B2" s="19" t="str">
         <f t="shared" ref="B2:B62" si="1">CONCATENATE(C2)</f>
         <v>Zürich</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="D2" s="5"/>
-      <c r="E2" s="5">
-        <v>2657896.0</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>648</v>
-      </c>
-      <c r="G2" s="8"/>
+      <c r="E2" s="7" t="s">
+        <v>649</v>
+      </c>
+      <c r="F2" s="8"/>
     </row>
     <row r="3" ht="22.5" customHeight="1">
       <c r="A3" s="3" t="s">
+        <v>650</v>
+      </c>
+      <c r="B3" s="19" t="str">
+        <f t="shared" si="1"/>
+        <v>Basel</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>651</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="7" t="s">
         <v>649</v>
       </c>
-      <c r="B3" s="19" t="str">
-        <f t="shared" si="1"/>
-        <v>Basel</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>650</v>
-      </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="7" t="s">
-        <v>648</v>
-      </c>
-      <c r="G3" s="8"/>
+      <c r="F3" s="8"/>
     </row>
     <row r="4" ht="22.5" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="B4" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Eidgenossenschaft</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="3" t="s">
-        <v>653</v>
+      <c r="E4" s="18"/>
+      <c r="F4" s="3" t="s">
+        <v>654</v>
       </c>
     </row>
     <row r="5" ht="22.5" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="B5" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Limmat</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="7" t="s">
-        <v>656</v>
-      </c>
-      <c r="G5" s="3" t="s">
+      <c r="E5" s="7" t="s">
         <v>657</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>658</v>
       </c>
     </row>
     <row r="6" ht="22.5" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="B6" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Weinfelden</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="8"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="8"/>
     </row>
     <row r="7" ht="22.5" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="B7" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Main (Fluss)</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="7" t="s">
-        <v>656</v>
-      </c>
-      <c r="G7" s="8"/>
+      <c r="E7" s="7" t="s">
+        <v>657</v>
+      </c>
+      <c r="F7" s="8"/>
     </row>
     <row r="8" ht="22.5" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="B8" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Zürichsee</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="7" t="s">
-        <v>656</v>
-      </c>
-      <c r="G8" s="8"/>
+      <c r="E8" s="7" t="s">
+        <v>657</v>
+      </c>
+      <c r="F8" s="8"/>
     </row>
     <row r="9" ht="22.5" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="B9" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Thalwil</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="3" t="s">
-        <v>666</v>
+      <c r="E9" s="13"/>
+      <c r="F9" s="3" t="s">
+        <v>667</v>
       </c>
     </row>
     <row r="10" ht="22.5" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="B10" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Bern</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="8"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="8"/>
     </row>
     <row r="11" ht="22.5" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="B11" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Gottstatt</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="8"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="8"/>
     </row>
     <row r="12" ht="22.5" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="B12" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Thorberg</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="8"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="8"/>
     </row>
     <row r="13" ht="22.5" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="B13" s="20" t="str">
         <f t="shared" si="1"/>
         <v>London</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="8"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="8"/>
     </row>
     <row r="14" ht="22.5" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="B14" s="20" t="str">
         <f t="shared" si="1"/>
         <v>England</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="8"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="8"/>
     </row>
     <row r="15" ht="22.5" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="B15" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Bethlehem</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="7" t="s">
-        <v>648</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>679</v>
+      <c r="E15" s="7" t="s">
+        <v>649</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>680</v>
       </c>
     </row>
     <row r="16" ht="22.5" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="B16" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Parnass (Berg)</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="7" t="s">
-        <v>682</v>
-      </c>
-      <c r="G16" s="6" t="s">
+      <c r="E16" s="7" t="s">
         <v>683</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>684</v>
       </c>
     </row>
     <row r="17" ht="22.5" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="B17" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Traubenberg</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="8"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="8"/>
     </row>
     <row r="18" ht="22.5" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="B18" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Babylon</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="7" t="s">
-        <v>648</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>688</v>
+      <c r="E18" s="7" t="s">
+        <v>649</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>689</v>
       </c>
     </row>
     <row r="19" ht="22.5" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="B19" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Canaan</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="3" t="s">
-        <v>691</v>
+      <c r="E19" s="13"/>
+      <c r="F19" s="3" t="s">
+        <v>692</v>
       </c>
     </row>
     <row r="20" ht="22.5" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="B20" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Ägypten</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="8"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="8"/>
     </row>
     <row r="21" ht="22.5" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="B21" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Hermon</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="7" t="s">
-        <v>682</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>696</v>
+      <c r="E21" s="7" t="s">
+        <v>683</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>697</v>
       </c>
     </row>
     <row r="22" ht="22.5" customHeight="1">
       <c r="A22" s="3" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="B22" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Jerusalem</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="8"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="8"/>
     </row>
     <row r="23" ht="22.5" customHeight="1">
       <c r="A23" s="3" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="B23" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Jordan</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="7" t="s">
-        <v>656</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>701</v>
+      <c r="E23" s="7" t="s">
+        <v>657</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>702</v>
       </c>
     </row>
     <row r="24" ht="22.5" customHeight="1">
       <c r="A24" s="3" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="B24" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Rotes Meer</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="7" t="s">
-        <v>656</v>
-      </c>
-      <c r="G24" s="8"/>
+      <c r="E24" s="7" t="s">
+        <v>657</v>
+      </c>
+      <c r="F24" s="8"/>
     </row>
     <row r="25" ht="22.5" customHeight="1">
       <c r="A25" s="3" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B25" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Juda</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="3" t="s">
-        <v>706</v>
+      <c r="E25" s="13"/>
+      <c r="F25" s="3" t="s">
+        <v>707</v>
       </c>
     </row>
     <row r="26" ht="22.5" customHeight="1">
       <c r="A26" s="3" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="B26" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Moab</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="3" t="s">
-        <v>709</v>
+      <c r="E26" s="13"/>
+      <c r="F26" s="3" t="s">
+        <v>710</v>
       </c>
     </row>
     <row r="27" ht="22.5" customHeight="1">
       <c r="A27" s="3" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="B27" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Ammon</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="3" t="s">
-        <v>712</v>
+      <c r="E27" s="13"/>
+      <c r="F27" s="3" t="s">
+        <v>713</v>
       </c>
     </row>
     <row r="28" ht="22.5" customHeight="1">
       <c r="A28" s="3" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="B28" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Zion</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="7" t="s">
-        <v>682</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>715</v>
+      <c r="E28" s="7" t="s">
+        <v>683</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>716</v>
       </c>
     </row>
     <row r="29" ht="22.5" customHeight="1">
       <c r="A29" s="3" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="B29" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Assur</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="3"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="3"/>
     </row>
     <row r="30" ht="22.5" customHeight="1">
       <c r="A30" s="3" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="B30" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Israel</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="3" t="s">
-        <v>720</v>
+      <c r="E30" s="13"/>
+      <c r="F30" s="3" t="s">
+        <v>721</v>
       </c>
     </row>
     <row r="31" ht="22.5" customHeight="1">
       <c r="A31" s="3" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="B31" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Nazaret</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="7" t="s">
-        <v>648</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>723</v>
+      <c r="E31" s="7" t="s">
+        <v>649</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>724</v>
       </c>
     </row>
     <row r="32" ht="22.5" customHeight="1">
       <c r="A32" s="3" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="B32" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Rom</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="3" t="s">
-        <v>726</v>
+      <c r="E32" s="13"/>
+      <c r="F32" s="3" t="s">
+        <v>727</v>
       </c>
     </row>
     <row r="33" ht="22.5" customHeight="1">
       <c r="A33" s="3" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="B33" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Samaria</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="3" t="s">
-        <v>729</v>
+      <c r="E33" s="13"/>
+      <c r="F33" s="3" t="s">
+        <v>730</v>
       </c>
     </row>
     <row r="34" ht="22.5" customHeight="1">
       <c r="A34" s="3" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="B34" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Kedronbach</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="3" t="s">
-        <v>732</v>
+      <c r="E34" s="13"/>
+      <c r="F34" s="3" t="s">
+        <v>733</v>
       </c>
     </row>
     <row r="35" ht="22.5" customHeight="1">
       <c r="A35" s="3" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="B35" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Garten von Getsemani</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="3"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="3"/>
     </row>
     <row r="36" ht="22.5" customHeight="1">
       <c r="A36" s="3" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="B36" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Urdorf</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="D36" s="21"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="3"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="3"/>
     </row>
     <row r="37" ht="22.5" customHeight="1">
       <c r="A37" s="3" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="B37" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Geiren-Rein</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="D37" s="21"/>
-      <c r="E37" s="21"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="3"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="3"/>
     </row>
     <row r="38" ht="22.5" customHeight="1">
       <c r="A38" s="3" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="B38" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Aeügst</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="D38" s="21"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="3"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="3"/>
     </row>
     <row r="39" ht="22.5" customHeight="1">
       <c r="A39" s="3" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="B39" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Riedt</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="D39" s="21"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="3"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="3"/>
     </row>
     <row r="40" ht="22.5" customHeight="1">
       <c r="A40" s="3" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="B40" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Europa</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="D40" s="21"/>
-      <c r="E40" s="21"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="3"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="3"/>
     </row>
     <row r="41" ht="22.5" customHeight="1">
       <c r="A41" s="3" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="B41" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Osir</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="D41" s="21"/>
-      <c r="E41" s="21"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="3" t="s">
-        <v>747</v>
+      <c r="E41" s="13"/>
+      <c r="F41" s="3" t="s">
+        <v>748</v>
       </c>
     </row>
     <row r="42" ht="22.5" customHeight="1">
       <c r="A42" s="3" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="B42" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Basadingen</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="3" t="s">
-        <v>750</v>
+      <c r="E42" s="13"/>
+      <c r="F42" s="3" t="s">
+        <v>751</v>
       </c>
     </row>
     <row r="43" ht="22.5" customHeight="1">
       <c r="A43" s="3" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="B43" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Diessenhofen</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="D43" s="21"/>
-      <c r="E43" s="21"/>
-      <c r="F43" s="13"/>
-      <c r="G43" s="3"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="3"/>
     </row>
     <row r="44" ht="22.5" customHeight="1">
       <c r="A44" s="3" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="B44" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Rhein</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="D44" s="21"/>
-      <c r="E44" s="21"/>
-      <c r="F44" s="7" t="s">
-        <v>656</v>
-      </c>
-      <c r="G44" s="3" t="s">
+      <c r="E44" s="7" t="s">
         <v>657</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>658</v>
       </c>
     </row>
     <row r="45" ht="22.5" customHeight="1">
       <c r="A45" s="3" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="B45" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Arabisches Reich</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="D45" s="21"/>
-      <c r="E45" s="21"/>
-      <c r="F45" s="13"/>
-      <c r="G45" s="3" t="s">
-        <v>757</v>
+      <c r="E45" s="13"/>
+      <c r="F45" s="3" t="s">
+        <v>758</v>
       </c>
     </row>
     <row r="46" ht="22.5" customHeight="1">
       <c r="A46" s="3" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="B46" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Libanon</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="D46" s="21"/>
-      <c r="E46" s="21"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="3"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="3"/>
     </row>
     <row r="47" ht="22.5" customHeight="1">
       <c r="A47" s="3" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="B47" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Emmaus</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="D47" s="21"/>
-      <c r="E47" s="21"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="3" t="s">
-        <v>762</v>
+      <c r="E47" s="13"/>
+      <c r="F47" s="3" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="48" ht="22.5" customHeight="1">
       <c r="A48" s="3" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="B48" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Helikon</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="D48" s="21"/>
-      <c r="E48" s="21"/>
-      <c r="F48" s="13"/>
-      <c r="G48" s="3" t="s">
-        <v>765</v>
+      <c r="E48" s="13"/>
+      <c r="F48" s="3" t="s">
+        <v>766</v>
       </c>
     </row>
     <row r="49" ht="22.5" customHeight="1">
       <c r="A49" s="3" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="B49" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Pindos</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="D49" s="21"/>
-      <c r="E49" s="21"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="3" t="s">
-        <v>768</v>
+      <c r="E49" s="13"/>
+      <c r="F49" s="3" t="s">
+        <v>769</v>
       </c>
     </row>
     <row r="50" ht="22.5" customHeight="1">
       <c r="A50" s="3" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="B50" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Neckar</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="D50" s="21"/>
-      <c r="E50" s="21"/>
-      <c r="F50" s="7" t="s">
-        <v>656</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>771</v>
+      <c r="E50" s="7" t="s">
+        <v>657</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>772</v>
       </c>
     </row>
     <row r="51" ht="22.5" customHeight="1">
       <c r="A51" s="3" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="B51" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Kurpfalz</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="D51" s="21"/>
-      <c r="E51" s="21"/>
-      <c r="F51" s="13"/>
-      <c r="G51" s="3" t="s">
-        <v>774</v>
+      <c r="E51" s="13"/>
+      <c r="F51" s="3" t="s">
+        <v>775</v>
       </c>
     </row>
     <row r="52" ht="22.5" customHeight="1">
       <c r="A52" s="3" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="B52" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Eglisau</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="D52" s="21"/>
-      <c r="E52" s="21"/>
-      <c r="F52" s="13"/>
-      <c r="G52" s="3"/>
+      <c r="E52" s="13"/>
+      <c r="F52" s="3"/>
     </row>
     <row r="53" ht="22.5" customHeight="1">
       <c r="A53" s="3" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="B53" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Altenklingen</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="D53" s="21"/>
-      <c r="E53" s="21"/>
-      <c r="F53" s="13"/>
-      <c r="G53" s="3"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="3"/>
     </row>
     <row r="54" ht="22.5" customHeight="1">
       <c r="A54" s="3" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="B54" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Altorff</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="D54" s="21"/>
-      <c r="E54" s="21"/>
-      <c r="F54" s="13"/>
-      <c r="G54" s="3"/>
+      <c r="E54" s="13"/>
+      <c r="F54" s="3"/>
     </row>
     <row r="55" ht="22.5" customHeight="1">
       <c r="A55" s="3" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="B55" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Glarus</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="D55" s="21"/>
-      <c r="E55" s="21"/>
-      <c r="F55" s="13"/>
-      <c r="G55" s="3"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="3"/>
     </row>
     <row r="56" ht="22.5" customHeight="1">
       <c r="A56" s="3" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="B56" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Bergerkirche</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="D56" s="21"/>
-      <c r="E56" s="21"/>
-      <c r="F56" s="13"/>
-      <c r="G56" s="3"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="3"/>
     </row>
     <row r="57" ht="22.5" customHeight="1">
       <c r="A57" s="3" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="B57" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Sodom</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="D57" s="21"/>
-      <c r="E57" s="21"/>
-      <c r="F57" s="13"/>
-      <c r="G57" s="3" t="s">
-        <v>787</v>
+      <c r="E57" s="13"/>
+      <c r="F57" s="3" t="s">
+        <v>788</v>
       </c>
     </row>
     <row r="58" ht="22.5" customHeight="1">
       <c r="A58" s="3" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="B58" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Haus zur Sonnenblume</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="D58" s="21"/>
-      <c r="E58" s="21"/>
-      <c r="F58" s="13"/>
-      <c r="G58" s="3"/>
+      <c r="E58" s="13"/>
+      <c r="F58" s="3"/>
     </row>
     <row r="59" ht="22.5" customHeight="1">
       <c r="A59" s="3" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="B59" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Thurn/ genennt von Geissen</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="D59" s="21"/>
-      <c r="E59" s="21"/>
-      <c r="F59" s="13"/>
-      <c r="G59" s="3" t="s">
-        <v>792</v>
+      <c r="E59" s="13"/>
+      <c r="F59" s="3" t="s">
+        <v>793</v>
       </c>
     </row>
     <row r="60" ht="22.5" customHeight="1">
       <c r="A60" s="3" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="B60" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Constantinopel</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="D60" s="21"/>
-      <c r="E60" s="21"/>
-      <c r="F60" s="13"/>
-      <c r="G60" s="3"/>
+      <c r="E60" s="13"/>
+      <c r="F60" s="3"/>
     </row>
     <row r="61" ht="22.5" customHeight="1">
       <c r="A61" s="3" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="B61" s="20" t="str">
         <f t="shared" si="1"/>
@@ -9391,13 +9336,12 @@
       </c>
       <c r="C61" s="3"/>
       <c r="D61" s="21"/>
-      <c r="E61" s="21"/>
-      <c r="F61" s="13"/>
-      <c r="G61" s="3"/>
+      <c r="E61" s="13"/>
+      <c r="F61" s="3"/>
     </row>
     <row r="62" ht="22.5" customHeight="1">
       <c r="A62" s="3" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="B62" s="20" t="str">
         <f t="shared" si="1"/>
@@ -9405,16 +9349,15 @@
       </c>
       <c r="C62" s="3"/>
       <c r="D62" s="21"/>
-      <c r="E62" s="21"/>
-      <c r="F62" s="13"/>
-      <c r="G62" s="3"/>
+      <c r="E62" s="13"/>
+      <c r="F62" s="3"/>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="F2:F62">
+    <dataValidation type="list" allowBlank="1" sqref="E2:E62">
       <formula1>"Stadt,Gewässer,Berg"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showDropDown="1" sqref="A2:A62 C2:C62 G2:G62"/>
+    <dataValidation allowBlank="1" showDropDown="1" sqref="A2:A62 C2:C62 F2:F62"/>
   </dataValidations>
   <drawing r:id="rId1"/>
   <tableParts count="1">
@@ -9449,25 +9392,25 @@
   <sheetData>
     <row r="1" ht="22.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>8</v>
@@ -9478,64 +9421,64 @@
     </row>
     <row r="2" ht="22.5" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="B2" s="22" t="str">
         <f t="shared" ref="B2:B20" si="1">CONCATENATE(C2)</f>
         <v>Teutsche Gedichte</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="I2" s="8"/>
     </row>
     <row r="3" ht="22.5" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="B3" s="22" t="str">
         <f t="shared" si="1"/>
         <v>Die Krafft der Gottseligkeit</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="23"/>
       <c r="G3" s="3"/>
       <c r="H3" s="7" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="I3" s="8"/>
     </row>
     <row r="4" ht="22.5" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="B4" s="22" t="str">
         <f t="shared" si="1"/>
         <v>Buch von Festen</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>588</v>
@@ -9548,17 +9491,17 @@
     </row>
     <row r="5" ht="22.5" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="B5" s="22" t="str">
         <f t="shared" si="1"/>
         <v>Psalm-Reimen und Melodien</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="21"/>
@@ -9568,17 +9511,17 @@
     </row>
     <row r="6" ht="22.5" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="B6" s="22" t="str">
         <f t="shared" si="1"/>
         <v>hundert Christliche/ neüaußgegebene Festpredigen</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="21"/>
@@ -9588,17 +9531,17 @@
     </row>
     <row r="7" ht="22.5" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="B7" s="22" t="str">
         <f t="shared" si="1"/>
         <v>Lehr- und trostreiche Predigen vom verlohrnen Sohn</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="21"/>
@@ -9608,17 +9551,17 @@
     </row>
     <row r="8" ht="22.5" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="B8" s="22" t="str">
         <f t="shared" si="1"/>
         <v>verteütschte Rueh- oder Fridens-uebung</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="21"/>
@@ -9628,17 +9571,17 @@
     </row>
     <row r="9" ht="22.5" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="B9" s="22" t="str">
         <f t="shared" si="1"/>
         <v>Nähefelser-Fahrt-Predigen</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="21"/>
@@ -9648,17 +9591,17 @@
     </row>
     <row r="10" ht="22.5" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="B10" s="22" t="str">
         <f t="shared" si="1"/>
         <v>Kinder-lehr</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="21"/>
@@ -9668,17 +9611,17 @@
     </row>
     <row r="11" ht="22.5" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="B11" s="22" t="str">
         <f t="shared" si="1"/>
         <v>neüaußgangenes Buech vom Vestungsbau</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="21"/>
@@ -9688,14 +9631,14 @@
     </row>
     <row r="12" ht="22.5" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="B12" s="22" t="str">
         <f t="shared" si="1"/>
         <v>Buech der Freunden Stammen</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="8"/>
@@ -9706,17 +9649,17 @@
     </row>
     <row r="13" ht="22.5" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="B13" s="22" t="str">
         <f t="shared" si="1"/>
         <v>Christen-spiegel</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="21"/>
@@ -9726,14 +9669,14 @@
     </row>
     <row r="14" ht="22.5" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="B14" s="22" t="str">
         <f t="shared" si="1"/>
         <v>Viergeticht</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="8"/>
@@ -9744,14 +9687,14 @@
     </row>
     <row r="15" ht="22.5" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="B15" s="22" t="str">
         <f t="shared" si="1"/>
         <v>Regentenspiegel</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="D15" s="21"/>
       <c r="E15" s="8"/>
@@ -9762,7 +9705,7 @@
     </row>
     <row r="16" ht="22.5" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="B16" s="22" t="str">
         <f t="shared" si="1"/>
@@ -9778,7 +9721,7 @@
     </row>
     <row r="17" ht="22.5" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="B17" s="22" t="str">
         <f t="shared" si="1"/>
@@ -9794,7 +9737,7 @@
     </row>
     <row r="18" ht="22.5" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="B18" s="22" t="str">
         <f t="shared" si="1"/>
@@ -9810,7 +9753,7 @@
     </row>
     <row r="19" ht="22.5" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="B19" s="22" t="str">
         <f t="shared" si="1"/>
@@ -9826,7 +9769,7 @@
     </row>
     <row r="20" ht="22.5" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="B20" s="22" t="str">
         <f t="shared" si="1"/>
@@ -9876,19 +9819,19 @@
   <sheetData>
     <row r="1" ht="22.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>10</v>
@@ -9896,69 +9839,69 @@
     </row>
     <row r="2" ht="22.5" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="B2" s="22" t="str">
         <f t="shared" ref="B2:B14" si="1">CONCATENATE(C2)</f>
         <v>Rat Zürich</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="D2" s="21"/>
       <c r="E2" s="24" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="F2" s="8"/>
     </row>
     <row r="3" ht="22.5" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="B3" s="22" t="str">
         <f t="shared" si="1"/>
         <v>Fruchtbringende Gesellschaft</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
     </row>
     <row r="4" ht="22.5" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="B4" s="22" t="str">
         <f t="shared" si="1"/>
         <v>Deutschgesinnte Genossenschaft</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="E4" s="13"/>
       <c r="F4" s="8"/>
     </row>
     <row r="5" ht="22.5" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="B5" s="22" t="str">
         <f t="shared" si="1"/>
         <v>Collegium Parthenicum</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="D5" s="16"/>
       <c r="E5" s="13"/>
@@ -9966,96 +9909,96 @@
     </row>
     <row r="6" ht="22.5" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="B6" s="22" t="str">
         <f t="shared" si="1"/>
         <v>Collegium Carolinum</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="8"/>
     </row>
     <row r="7" ht="22.5" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="B7" s="22" t="str">
         <f t="shared" si="1"/>
         <v>Sanhedrin</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="D7" s="16"/>
       <c r="E7" s="13"/>
       <c r="F7" s="3" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
     </row>
     <row r="8" ht="22.5" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="B8" s="22" t="str">
         <f t="shared" si="1"/>
         <v>Stadtbibliothek Zürich</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="D8" s="16"/>
       <c r="E8" s="13"/>
       <c r="F8" s="3" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
     </row>
     <row r="9" ht="22.5" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="B9" s="22" t="str">
         <f t="shared" si="1"/>
         <v>Grossmünster</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="3" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
     </row>
     <row r="10" ht="22.5" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="B10" s="22" t="str">
         <f t="shared" si="1"/>
         <v>Fraumünster</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="3" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
     </row>
     <row r="11" ht="22.5" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="B11" s="22" t="str">
         <f t="shared" si="1"/>
@@ -10068,7 +10011,7 @@
     </row>
     <row r="12" ht="22.5" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="B12" s="22" t="str">
         <f t="shared" si="1"/>
@@ -10081,7 +10024,7 @@
     </row>
     <row r="13" ht="22.5" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="B13" s="22" t="str">
         <f t="shared" si="1"/>
@@ -10094,7 +10037,7 @@
     </row>
     <row r="14" ht="22.5" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="B14" s="22" t="str">
         <f t="shared" si="1"/>
@@ -10141,19 +10084,19 @@
   <sheetData>
     <row r="1" ht="22.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>10</v>
@@ -10161,26 +10104,26 @@
     </row>
     <row r="2" ht="22.5" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="B2" s="19" t="str">
         <f t="shared" ref="B2:B8" si="1">CONCATENATE(C2)</f>
         <v>Runs</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="F2" s="8"/>
     </row>
     <row r="3" ht="22.5" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="B3" s="19" t="str">
         <f t="shared" si="1"/>
@@ -10193,7 +10136,7 @@
     </row>
     <row r="4" ht="22.5" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="B4" s="19" t="str">
         <f t="shared" si="1"/>
@@ -10206,7 +10149,7 @@
     </row>
     <row r="5" ht="22.5" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="B5" s="19" t="str">
         <f t="shared" si="1"/>
@@ -10219,7 +10162,7 @@
     </row>
     <row r="6" ht="22.5" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="B6" s="19" t="str">
         <f t="shared" si="1"/>
@@ -10232,7 +10175,7 @@
     </row>
     <row r="7" ht="22.5" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="B7" s="19" t="str">
         <f t="shared" si="1"/>
@@ -10245,7 +10188,7 @@
     </row>
     <row r="8" ht="22.5" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="B8" s="19" t="str">
         <f t="shared" si="1"/>

</xml_diff>